<commit_message>
updated and saved phyloseq files. added zaids code for aggregating taxa
</commit_message>
<xml_diff>
--- a/excel sheets/Cow_map_wrichness.xlsx
+++ b/excel sheets/Cow_map_wrichness.xlsx
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B142" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>